<commit_message>
development on diminishing list
</commit_message>
<xml_diff>
--- a/frontend/vbal.xlsx
+++ b/frontend/vbal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\ProjVb\frontend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\ProjVerb\frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C524959-7E2A-4366-AE72-2684332D6905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E6CF21-DC83-455A-A5F6-2053B77651A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0E7A44A2-6AA7-4951-8310-C2003754AB33}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>abbeißen</t>
   </si>
@@ -109,9 +109,6 @@
     <t>transmettre, restituer</t>
   </si>
   <si>
-    <t>se déhabituer</t>
-  </si>
-  <si>
     <t>délimiter</t>
   </si>
   <si>
@@ -134,13 +131,19 @@
   </si>
   <si>
     <t>Verbe Francais 4</t>
+  </si>
+  <si>
+    <t>se déshabituer</t>
+  </si>
+  <si>
+    <t>se résigner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +152,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -175,8 +187,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -494,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4167B49E-280D-4F97-A16F-747FF3B53422}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -509,19 +522,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -574,6 +587,9 @@
       <c r="B7" t="s">
         <v>20</v>
       </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -612,7 +628,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -620,7 +636,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -628,7 +644,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -636,7 +652,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>